<commit_message>
Lab 1 and 2
</commit_message>
<xml_diff>
--- a/Result/MethOpt.xlsx
+++ b/Result/MethOpt.xlsx
@@ -7,15 +7,17 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Laba1" sheetId="1" r:id="rId1"/>
-    <sheet name="Laba2" sheetId="2" r:id="rId2"/>
+    <sheet name="Lab1_1" sheetId="1" r:id="rId1"/>
+    <sheet name="Lab1_2" sheetId="2" r:id="rId2"/>
+    <sheet name="Lab2_1" sheetId="3" r:id="rId3"/>
+    <sheet name="Lab2_2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="154">
   <si>
     <t>x</t>
   </si>
@@ -32,241 +34,451 @@
     <t>alpha</t>
   </si>
   <si>
-    <t>[ 0.  0.  0.]</t>
-  </si>
-  <si>
     <t>[-0.0625  0.      0.0625]</t>
   </si>
   <si>
-    <t>[  0.00000000e+00   7.03125000e-05   1.09375000e-01]</t>
-  </si>
-  <si>
-    <t>[ -6.25000791e-02  -6.15234375e-05   1.44531250e-01]</t>
-  </si>
-  <si>
-    <t>[  1.48315430e-07   1.24145597e-04   1.70898438e-01]</t>
-  </si>
-  <si>
-    <t>[ -6.25002880e-02  -1.08627564e-04   1.90673828e-01]</t>
-  </si>
-  <si>
-    <t>[  4.10185236e-07   1.65361943e-04   2.05505371e-01]</t>
-  </si>
-  <si>
-    <t>[ -6.25005962e-02  -1.44692161e-04   2.16629028e-01]</t>
-  </si>
-  <si>
-    <t>[  7.58996102e-07   1.96918812e-04   2.24971771e-01]</t>
-  </si>
-  <si>
-    <t>[ -6.25009805e-02  -1.72304814e-04   2.31228828e-01]</t>
-  </si>
-  <si>
-    <t>[  1.17437268e-06   2.21080315e-04   2.35921621e-01]</t>
-  </si>
-  <si>
-    <t>[ -6.25014231e-02  -1.93446597e-04   2.39441216e-01]</t>
-  </si>
-  <si>
-    <t>[  1.64071546e-06   2.39579874e-04   2.42080912e-01]</t>
-  </si>
-  <si>
-    <t>[ -6.25019102e-02  -2.09634235e-04   2.44060684e-01]</t>
-  </si>
-  <si>
-    <t>[  2.14608133e-06   2.53744605e-04   2.45545513e-01]</t>
-  </si>
-  <si>
-    <t>[ -6.25024315e-02  -2.22028944e-04   2.46659135e-01]</t>
-  </si>
-  <si>
-    <t>[  2.68132657e-06   2.64590561e-04   2.47494351e-01]</t>
-  </si>
-  <si>
-    <t>[ -6.25029790e-02  -2.31519757e-04   2.48120763e-01]</t>
-  </si>
-  <si>
-    <t>[  3.23945068e-06   2.72895639e-04   2.48590572e-01]</t>
-  </si>
-  <si>
-    <t>[ -6.25035465e-02  -2.38787329e-04   2.48942929e-01]</t>
-  </si>
-  <si>
-    <t>[  3.81509402e-06   2.79255402e-04   2.49207197e-01]</t>
-  </si>
-  <si>
-    <t>[ -6.25041293e-02  -2.44352769e-04   2.49405398e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12498626e-02   1.98865246e-05   2.49479723e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12510516e-02   1.13619713e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12489612e-02   2.52157082e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12510672e-02   1.30913366e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12489475e-02   2.37025311e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12510792e-02   1.44153513e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12489371e-02   2.25440317e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12510883e-02   1.54290265e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12489291e-02   2.16570762e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12510953e-02   1.62051035e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12489229e-02   2.09780166e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12511007e-02   1.67992738e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12489182e-02   2.04581237e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12511048e-02   1.72541748e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12489146e-02   2.00600900e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12511079e-02   1.76024502e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12489119e-02   1.97553525e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12511104e-02   1.78690924e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12489097e-02   1.95220433e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12511122e-02   1.80732356e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12489081e-02   1.93434201e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12511137e-02   1.82295290e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12489069e-02   1.92066650e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12511148e-02   1.83491883e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12489059e-02   1.91019643e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12511156e-02   1.84408004e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12489051e-02   1.90218047e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12511163e-02   1.85109391e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12489046e-02   1.89604340e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12511168e-02   1.85646379e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12489041e-02   1.89134482e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12511172e-02   1.86057499e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12489038e-02   1.88774756e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12511175e-02   1.86372256e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12489035e-02   1.88499347e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12511177e-02   1.86613235e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12489033e-02   1.88288493e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12511179e-02   1.86797731e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12489031e-02   1.88127062e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12511180e-02   1.86938981e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12489030e-02   1.88003470e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12511182e-02   1.87047123e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12489029e-02   1.87908847e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12511183e-02   1.87129917e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12489028e-02   1.87836403e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12511183e-02   1.87193304e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12489027e-02   1.87780941e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12511184e-02   1.87241833e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12489027e-02   1.87738478e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12511185e-02   1.87278986e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12489026e-02   1.87705970e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12511185e-02   1.87307431e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12500105e-02   1.87494256e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12500106e-02   1.87516033e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12500000e-02   1.87500000e-06   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12500011e-02   1.87500001e-05   2.50000000e-01]</t>
-  </si>
-  <si>
-    <t>[ -3.12500105e-02   1.87500012e-05   2.50000000e-01]</t>
+    <t>[1.79722903e-12 7.03125015e-05 1.09375000e-01]</t>
+  </si>
+  <si>
+    <t>[-6.25000791e-02 -6.15234426e-05  1.44531250e-01]</t>
+  </si>
+  <si>
+    <t>[1.48320654e-07 1.24145607e-04 1.70898438e-01]</t>
+  </si>
+  <si>
+    <t>[-6.25002880e-02 -1.08627577e-04  1.90673828e-01]</t>
+  </si>
+  <si>
+    <t>[4.10198847e-07 1.65361952e-04 2.05505371e-01]</t>
+  </si>
+  <si>
+    <t>[-6.25005962e-02 -1.44692171e-04  2.16629028e-01]</t>
+  </si>
+  <si>
+    <t>[7.59012707e-07 1.96918822e-04 2.24971771e-01]</t>
+  </si>
+  <si>
+    <t>[-6.25009805e-02 -1.72304822e-04  2.31228828e-01]</t>
+  </si>
+  <si>
+    <t>[1.17439658e-06 2.21080329e-04 2.35921621e-01]</t>
+  </si>
+  <si>
+    <t>[-6.25014231e-02 -1.93446609e-04  2.39441216e-01]</t>
+  </si>
+  <si>
+    <t>[1.64074229e-06 2.39579879e-04 2.42080912e-01]</t>
+  </si>
+  <si>
+    <t>[-6.25019103e-02 -2.09634241e-04  2.44060684e-01]</t>
+  </si>
+  <si>
+    <t>[2.14610627e-06 2.53744608e-04 2.45545513e-01]</t>
+  </si>
+  <si>
+    <t>[-6.25024316e-02 -2.22028949e-04  2.46659135e-01]</t>
+  </si>
+  <si>
+    <t>[2.68135520e-06 2.64590563e-04 2.47494351e-01]</t>
+  </si>
+  <si>
+    <t>[-6.25029790e-02 -2.31519760e-04  2.48120763e-01]</t>
+  </si>
+  <si>
+    <t>[3.23948513e-06 2.72895638e-04 2.48590572e-01]</t>
+  </si>
+  <si>
+    <t>[-6.25035465e-02 -2.38787328e-04  2.48942929e-01]</t>
+  </si>
+  <si>
+    <t>[3.81513577e-06 2.79255408e-04 2.49207197e-01]</t>
+  </si>
+  <si>
+    <t>[-6.25041293e-02 -2.44352776e-04  2.49405398e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12498625e-02  1.98865230e-05  2.49479723e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12510517e-02  1.13619877e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12489611e-02  2.52156976e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12510673e-02  1.30913509e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12489475e-02  2.37025156e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12510792e-02  1.44153613e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12489370e-02  2.25440239e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12510883e-02  1.54290296e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12489290e-02  2.16570685e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12510953e-02  1.62051102e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12489229e-02  2.09780110e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12511007e-02  1.67992790e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12489182e-02  2.04581144e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12511048e-02  1.72541842e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12489146e-02  2.00600821e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.1251108e-02  1.7602456e-05  2.5000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12489118e-02  1.97553432e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12511104e-02  1.78691003e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12489097e-02  1.95220402e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12511123e-02  1.80732339e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12489081e-02  1.93434158e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12511137e-02  1.82295325e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12489068e-02  1.92066675e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12511148e-02  1.83491850e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12489058e-02  1.91019683e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12511157e-02  1.84408044e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12489051e-02  1.90217980e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12511163e-02  1.85109480e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12489045e-02  1.89604235e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12511168e-02  1.85646463e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12489041e-02  1.89134385e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12511172e-02  1.86057593e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12489037e-02  1.88774690e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12511175e-02  1.86372272e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12489034e-02  1.88499303e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12511178e-02  1.86613225e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12489032e-02  1.88288534e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12511180e-02  1.86797626e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12489030e-02  1.88127205e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12511181e-02  1.86938832e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12489029e-02  1.88003606e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12511182e-02  1.87046992e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12489028e-02  1.87908890e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12511183e-02  1.87129912e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12489027e-02  1.87836378e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12511184e-02  1.87193316e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12489026e-02  1.87780867e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12511185e-02  1.87241889e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12489026e-02  1.87738367e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12511186e-02  1.87279098e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12489025e-02  1.87705840e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12500106e-02  1.87506694e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12500105e-02  1.87494291e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-0.05555549  0.          0.05555549]</t>
+  </si>
+  <si>
+    <t>[-1.23457311e-02  5.55554869e-05  9.87653800e-02]</t>
+  </si>
+  <si>
+    <t>[-4.59532543e-02 -2.46909696e-05  1.32372952e-01]</t>
+  </si>
+  <si>
+    <t>[-1.98141582e-02  6.24137409e-05  1.58512249e-01]</t>
+  </si>
+  <si>
+    <t>[-4.01445080e-02 -2.17945963e-05  1.78842762e-01]</t>
+  </si>
+  <si>
+    <t>[-2.43320656e-02  5.46740505e-05  1.94655443e-01]</t>
+  </si>
+  <si>
+    <t>[-3.66306110e-02 -1.21169838e-05  2.06954174e-01]</t>
+  </si>
+  <si>
+    <t>[-2.70650913e-02  4.47084651e-05  2.16519890e-01]</t>
+  </si>
+  <si>
+    <t>[-3.45049288e-02 -2.74026116e-06  2.23959870e-01]</t>
+  </si>
+  <si>
+    <t>[-2.87183999e-02  3.63316773e-05  2.29746552e-01]</t>
+  </si>
+  <si>
+    <t>[-3.32190315e-02  4.49747295e-06  2.34247291e-01]</t>
+  </si>
+  <si>
+    <t>[-2.97185419e-02  3.02206694e-05  2.37747886e-01]</t>
+  </si>
+  <si>
+    <t>[-3.24411413e-02  9.57160518e-06  2.40470555e-01]</t>
+  </si>
+  <si>
+    <t>[-3.03235663e-02  2.60600747e-05  2.42588210e-01]</t>
+  </si>
+  <si>
+    <t>[-3.19705727e-02  1.29502862e-05  2.44235261e-01]</t>
+  </si>
+  <si>
+    <t>[-3.06895706e-02  2.33370298e-05  2.45516311e-01]</t>
+  </si>
+  <si>
+    <t>[-3.16859081e-02  1.51315806e-05  2.46512682e-01]</t>
+  </si>
+  <si>
+    <t>[-3.09109811e-02  2.15981357e-05  2.47287636e-01]</t>
+  </si>
+  <si>
+    <t>[-3.15137037e-02  1.65122211e-05  2.47890384e-01]</t>
+  </si>
+  <si>
+    <t>[-3.10449193e-02  2.05055064e-05  2.48359182e-01]</t>
+  </si>
+  <si>
+    <t>[-3.14095292e-02  1.73745717e-05  2.48723810e-01]</t>
+  </si>
+  <si>
+    <t>[-3.11259437e-02  1.98264439e-05  2.49007403e-01]</t>
+  </si>
+  <si>
+    <t>[-3.13465102e-02  1.79082993e-05  2.49227982e-01]</t>
+  </si>
+  <si>
+    <t>[-3.11749590e-02  1.94076003e-05  2.49399537e-01]</t>
+  </si>
+  <si>
+    <t>[-3.13083864e-02  1.82365462e-05  2.49532975e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12046085e-02  1.91506744e-05  2.49636756e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12853246e-02  1.84374867e-05  2.49717478e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12225463e-02  1.89936401e-05  2.49780258e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12713744e-02  1.85600989e-05  2.49829092e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12333972e-02  1.88979487e-05  2.49867069e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12629350e-02  1.86347389e-05  2.49896612e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12399603e-02  1.88397556e-05  2.49919585e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12578288e-02  1.86801111e-05  2.49937456e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12439319e-02  1.88043975e-05  2.49951352e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12547405e-02  1.87076508e-05  2.49962165e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12463327e-02  1.87829671e-05  2.49970572e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12528706e-02  1.87243618e-05  2.49977111e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12477856e-02  1.87699621e-05  2.49982198e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12517404e-02  1.87344877e-05  2.49986153e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12486652e-02  1.87620806e-05  2.49989230e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12510575e-02  1.87406037e-05  2.49991624e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12491955e-02  1.87573257e-05  2.49993486e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12506429e-02  1.87443260e-05  2.49994932e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12495185e-02  1.87544285e-05  2.49996058e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12503932e-02  1.87465651e-05  2.49996934e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12497132e-02  1.87526844e-05  2.49997615e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12502417e-02  1.87479207e-05  2.49998145e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12498310e-02  1.87516274e-05  2.49998557e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12501508e-02  1.87487392e-05  2.49998878e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12499027e-02  1.87509799e-05  2.49999126e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12500950e-02  1.87492483e-05  2.49999321e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12499454e-02  1.87505853e-05  2.49999471e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12500620e-02  1.87495453e-05  2.49999590e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12499720e-02  1.87503498e-05  2.49999679e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12500419e-02  1.87497289e-05  2.49999752e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12499880e-02  1.87502065e-05  2.49999805e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12500297e-02  1.87498378e-05  2.49999850e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12499959e-02  1.87501364e-05  2.49999883e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12500216e-02  1.87499083e-05  2.49999909e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12500019e-02  1.87500867e-05  2.49999929e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12500168e-02  1.87499528e-05  2.49999944e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12500057e-02  1.87500458e-05  2.49999957e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12500139e-02  1.87499802e-05  2.49999966e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12500080e-02  1.87500267e-05  2.49999973e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12500132e-02  1.87499823e-05  2.49999980e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12500096e-02  1.87500118e-05  2.49999984e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12500123e-02  1.87499877e-05  2.49999989e-01]</t>
+  </si>
+  <si>
+    <t>[-3.125e-02  1.875e-12  2.500e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12500000e-02  1.87511075e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12500105e-02  1.87500021e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12500105e-02  1.87500067e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12499958e-02  1.87499975e-12  2.49999966e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12500000e-02  1.87498591e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12500086e-02  1.87499767e-05  2.50000000e-01]</t>
+  </si>
+  <si>
+    <t>[-3.12500100e-02  1.87499969e-05  2.50000000e-01]</t>
   </si>
 </sst>
 </file>
@@ -624,7 +836,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F77"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -655,16 +867,16 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>1.414213562373095</v>
+        <v>1.4142135623731</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>-0.0546875</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.0883883476483184</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.0625</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -675,13 +887,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>1.414213562373095</v>
+        <v>1.25000050628586</v>
       </c>
       <c r="D3">
-        <v>-0.05468750000000001</v>
+        <v>-0.085449144591243</v>
       </c>
       <c r="E3">
-        <v>0.08838834764831843</v>
+        <v>0.0781250316428665</v>
       </c>
       <c r="F3">
         <v>0.0625</v>
@@ -695,13 +907,13 @@
         <v>7</v>
       </c>
       <c r="C4">
-        <v>1.250000506249898</v>
+        <v>1.14735052659951</v>
       </c>
       <c r="D4">
-        <v>-0.08544914459228516</v>
+        <v>-0.102752480454324</v>
       </c>
       <c r="E4">
-        <v>0.07812503164061858</v>
+        <v>0.0717094079124694</v>
       </c>
       <c r="F4">
         <v>0.0625</v>
@@ -715,13 +927,13 @@
         <v>8</v>
       </c>
       <c r="C5">
-        <v>1.147350526523822</v>
+        <v>1.08535460486311</v>
       </c>
       <c r="D5">
-        <v>-0.1027524804542572</v>
+        <v>-0.112485506118304</v>
       </c>
       <c r="E5">
-        <v>0.0717094079077389</v>
+        <v>0.0678346628039446</v>
       </c>
       <c r="F5">
         <v>0.0625</v>
@@ -735,13 +947,13 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>1.08535460475713</v>
+        <v>1.04887594492644</v>
       </c>
       <c r="D6">
-        <v>-0.112485506122066</v>
+        <v>-0.117960223469783</v>
       </c>
       <c r="E6">
-        <v>0.06783466279732063</v>
+        <v>0.0655547465579023</v>
       </c>
       <c r="F6">
         <v>0.0625</v>
@@ -755,13 +967,13 @@
         <v>10</v>
       </c>
       <c r="C7">
-        <v>1.04887594473939</v>
+        <v>1.02779135760194</v>
       </c>
       <c r="D7">
-        <v>-0.1179602234749752</v>
+        <v>-0.121039635627416</v>
       </c>
       <c r="E7">
-        <v>0.06555474654621186</v>
+        <v>0.0642369598501211</v>
       </c>
       <c r="F7">
         <v>0.0625</v>
@@ -775,13 +987,13 @@
         <v>11</v>
       </c>
       <c r="C8">
-        <v>1.027791357270997</v>
+        <v>1.0157426683422</v>
       </c>
       <c r="D8">
-        <v>-0.1210396356392611</v>
+        <v>-0.122771683443077</v>
       </c>
       <c r="E8">
-        <v>0.06423695982943732</v>
+        <v>0.0634839167713873</v>
       </c>
       <c r="F8">
         <v>0.0625</v>
@@ -795,13 +1007,13 @@
         <v>12</v>
       </c>
       <c r="C9">
-        <v>1.015742667882209</v>
+        <v>1.00890593764751</v>
       </c>
       <c r="D9">
-        <v>-0.1227716834576417</v>
+        <v>-0.123745834850393</v>
       </c>
       <c r="E9">
-        <v>0.06348391674263806</v>
+        <v>0.0630566211029691</v>
       </c>
       <c r="F9">
         <v>0.0625</v>
@@ -815,13 +1027,13 @@
         <v>13</v>
       </c>
       <c r="C10">
-        <v>1.008905937151234</v>
+        <v>1.00504386071473</v>
       </c>
       <c r="D10">
-        <v>-0.1237458348670114</v>
+        <v>-0.124293666492105</v>
       </c>
       <c r="E10">
-        <v>0.06305662107195213</v>
+        <v>0.0628152412946707</v>
       </c>
       <c r="F10">
         <v>0.0625</v>
@@ -835,13 +1047,13 @@
         <v>14</v>
       </c>
       <c r="C11">
-        <v>1.00504386015638</v>
+        <v>1.00286902734505</v>
       </c>
       <c r="D11">
-        <v>-0.124293666510452</v>
+        <v>-0.124601690936557</v>
       </c>
       <c r="E11">
-        <v>0.06281524125977377</v>
+        <v>0.0626793142090659</v>
       </c>
       <c r="F11">
         <v>0.0625</v>
@@ -855,13 +1067,13 @@
         <v>15</v>
       </c>
       <c r="C12">
-        <v>1.002869026671455</v>
+        <v>1.00164780389076</v>
       </c>
       <c r="D12">
-        <v>-0.1246016909606235</v>
+        <v>-0.124774822061008</v>
       </c>
       <c r="E12">
-        <v>0.06267931416696591</v>
+        <v>0.0626029877431727</v>
       </c>
       <c r="F12">
         <v>0.0625</v>
@@ -875,13 +1087,13 @@
         <v>16</v>
       </c>
       <c r="C13">
-        <v>1.001647803144798</v>
+        <v>1.00096446263866</v>
       </c>
       <c r="D13">
-        <v>-0.1247748220839376</v>
+        <v>-0.124872074319818</v>
       </c>
       <c r="E13">
-        <v>0.06260298769654987</v>
+        <v>0.0625602789149161</v>
       </c>
       <c r="F13">
         <v>0.0625</v>
@@ -895,13 +1107,13 @@
         <v>17</v>
       </c>
       <c r="C14">
-        <v>1.000964461848257</v>
+        <v>1.00058417234998</v>
       </c>
       <c r="D14">
-        <v>-0.1248720743469637</v>
+        <v>-0.124926643680042</v>
       </c>
       <c r="E14">
-        <v>0.06256027886551607</v>
+        <v>0.062536510771874</v>
       </c>
       <c r="F14">
         <v>0.0625</v>
@@ -915,13 +1127,13 @@
         <v>18</v>
       </c>
       <c r="C15">
-        <v>1.000584171501366</v>
+        <v>1.00037452192696</v>
       </c>
       <c r="D15">
-        <v>-0.1249266437061856</v>
+        <v>-0.124957203106408</v>
       </c>
       <c r="E15">
-        <v>0.06253651071883536</v>
+        <v>0.0625234076204347</v>
       </c>
       <c r="F15">
         <v>0.0625</v>
@@ -935,13 +1147,13 @@
         <v>19</v>
       </c>
       <c r="C16">
-        <v>1.000374521109722</v>
+        <v>1.00026092524766</v>
       </c>
       <c r="D16">
-        <v>-0.1249572031313832</v>
+        <v>-0.124974256328458</v>
       </c>
       <c r="E16">
-        <v>0.06252340756935762</v>
+        <v>0.0625163078279785</v>
       </c>
       <c r="F16">
         <v>0.0625</v>
@@ -955,13 +1167,13 @@
         <v>20</v>
       </c>
       <c r="C17">
-        <v>1.000260924422659</v>
+        <v>1.00020139113902</v>
       </c>
       <c r="D17">
-        <v>-0.1249742563550636</v>
+        <v>-0.124983711841302</v>
       </c>
       <c r="E17">
-        <v>0.06251630777641617</v>
+        <v>0.0625125869461889</v>
       </c>
       <c r="F17">
         <v>0.0625</v>
@@ -975,13 +1187,13 @@
         <v>21</v>
       </c>
       <c r="C18">
-        <v>1.000201390254918</v>
+        <v>1.0001722855869</v>
       </c>
       <c r="D18">
-        <v>-0.124983711869935</v>
+        <v>-0.124988893280445</v>
       </c>
       <c r="E18">
-        <v>0.06251258689093235</v>
+        <v>0.0625107678491812</v>
       </c>
       <c r="F18">
         <v>0.0625</v>
@@ -995,13 +1207,13 @@
         <v>22</v>
       </c>
       <c r="C19">
-        <v>1.000172284610662</v>
+        <v>1.00016030814589</v>
       </c>
       <c r="D19">
-        <v>-0.1249888933127598</v>
+        <v>-0.124991670278704</v>
       </c>
       <c r="E19">
-        <v>0.06251076778816637</v>
+        <v>0.062510019259118</v>
       </c>
       <c r="F19">
         <v>0.0625</v>
@@ -1015,13 +1227,13 @@
         <v>23</v>
       </c>
       <c r="C20">
-        <v>1.000160307077551</v>
+        <v>1.00015797387181</v>
       </c>
       <c r="D20">
-        <v>-0.1249916703131385</v>
+        <v>-0.124993094565561</v>
       </c>
       <c r="E20">
-        <v>0.06251001919234693</v>
+        <v>0.0625098733669879</v>
       </c>
       <c r="F20">
         <v>0.0625</v>
@@ -1035,13 +1247,13 @@
         <v>24</v>
       </c>
       <c r="C21">
-        <v>1.000157972738286</v>
+        <v>1.00016107037849</v>
       </c>
       <c r="D21">
-        <v>-0.1249930946019722</v>
+        <v>-0.124993757785285</v>
       </c>
       <c r="E21">
-        <v>0.06250987329614285</v>
+        <v>0.0625100668986558</v>
       </c>
       <c r="F21">
         <v>0.0625</v>
@@ -1055,13 +1267,13 @@
         <v>25</v>
       </c>
       <c r="C22">
-        <v>1.000161069127214</v>
+        <v>1.00016722656596</v>
       </c>
       <c r="D22">
-        <v>-0.1249937578270836</v>
+        <v>-0.124993992783246</v>
       </c>
       <c r="E22">
-        <v>0.0625100668204509</v>
+        <v>0.0625104516603725</v>
       </c>
       <c r="F22">
         <v>0.0625</v>
@@ -1075,16 +1287,16 @@
         <v>26</v>
       </c>
       <c r="C23">
-        <v>1.000167225180922</v>
+        <v>1.00017510756547</v>
       </c>
       <c r="D23">
-        <v>-0.1249939928280339</v>
+        <v>-0.140624463877475</v>
       </c>
       <c r="E23">
-        <v>0.06251045157380763</v>
+        <v>0.0312554721114211</v>
       </c>
       <c r="F23">
-        <v>0.0625</v>
+        <v>0.03125</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1095,16 +1307,16 @@
         <v>27</v>
       </c>
       <c r="C24">
-        <v>1.000175106028308</v>
+        <v>0.00208139268333609</v>
       </c>
       <c r="D24">
-        <v>-0.1406244638774831</v>
+        <v>-0.140625004437216</v>
       </c>
       <c r="E24">
-        <v>0.03125547206338464</v>
+        <v>0.000520348170834022</v>
       </c>
       <c r="F24">
-        <v>0.03125</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1115,16 +1327,16 @@
         <v>28</v>
       </c>
       <c r="C25">
-        <v>0.002081392594203371</v>
+        <v>0.000224168893820515</v>
       </c>
       <c r="D25">
-        <v>-0.1406250044372133</v>
+        <v>-0.140625004628619</v>
       </c>
       <c r="E25">
-        <v>0.0005203481485508532</v>
+        <v>1.40105558637822e-05</v>
       </c>
       <c r="F25">
-        <v>0.25</v>
+        <v>0.0625</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1135,13 +1347,13 @@
         <v>29</v>
       </c>
       <c r="C26">
-        <v>0.0002241691419935607</v>
+        <v>0.000196894671729243</v>
       </c>
       <c r="D26">
-        <v>-0.140625004628618</v>
+        <v>-0.14062500477516</v>
       </c>
       <c r="E26">
-        <v>1.401057137459754e-05</v>
+        <v>1.23059169830777e-05</v>
       </c>
       <c r="F26">
         <v>0.0625</v>
@@ -1155,13 +1367,13 @@
         <v>30</v>
       </c>
       <c r="C27">
-        <v>0.0001968948551786942</v>
+        <v>0.000173133195419566</v>
       </c>
       <c r="D27">
-        <v>-0.1406250047751588</v>
+        <v>-0.140625004887353</v>
       </c>
       <c r="E27">
-        <v>1.230592844866779e-05</v>
+        <v>1.08208247137229e-05</v>
       </c>
       <c r="F27">
         <v>0.0625</v>
@@ -1175,13 +1387,13 @@
         <v>31</v>
       </c>
       <c r="C28">
-        <v>0.0001731334378889046</v>
+        <v>0.000152458599193128</v>
       </c>
       <c r="D28">
-        <v>-0.1406250048873514</v>
+        <v>-0.140625004973247</v>
       </c>
       <c r="E28">
-        <v>1.082083986805654e-05</v>
+        <v>9.52866244957048e-06</v>
       </c>
       <c r="F28">
         <v>0.0625</v>
@@ -1195,13 +1407,13 @@
         <v>32</v>
       </c>
       <c r="C29">
-        <v>0.0001524587496523138</v>
+        <v>0.000134499008927613</v>
       </c>
       <c r="D29">
-        <v>-0.1406250049732468</v>
+        <v>-0.140625005039008</v>
       </c>
       <c r="E29">
-        <v>9.528671853270391e-06</v>
+        <v>8.40618805797579e-06</v>
       </c>
       <c r="F29">
         <v>0.0625</v>
@@ -1215,13 +1427,13 @@
         <v>33</v>
       </c>
       <c r="C30">
-        <v>0.0001344989884414661</v>
+        <v>0.000118929920710781</v>
       </c>
       <c r="D30">
-        <v>-0.1406250050390088</v>
+        <v>-0.140625005089355</v>
       </c>
       <c r="E30">
-        <v>8.406186777591629e-06</v>
+        <v>7.43312004442381e-06</v>
       </c>
       <c r="F30">
         <v>0.0625</v>
@@ -1235,13 +1447,13 @@
         <v>34</v>
       </c>
       <c r="C31">
-        <v>0.0001189297245351933</v>
+        <v>0.000105467926395962</v>
       </c>
       <c r="D31">
-        <v>-0.1406250050893565</v>
+        <v>-0.140625005127902</v>
       </c>
       <c r="E31">
-        <v>7.433107783448575e-06</v>
+        <v>6.5917453997476e-06</v>
       </c>
       <c r="F31">
         <v>0.0625</v>
@@ -1255,13 +1467,13 @@
         <v>35</v>
       </c>
       <c r="C32">
-        <v>0.0001054676719306169</v>
+        <v>9.38652869380353e-05</v>
       </c>
       <c r="D32">
-        <v>-0.1406250051279031</v>
+        <v>-0.140625005157414</v>
       </c>
       <c r="E32">
-        <v>6.591729495663556e-06</v>
+        <v>5.86658043362721e-06</v>
       </c>
       <c r="F32">
         <v>0.0625</v>
@@ -1275,13 +1487,13 @@
         <v>36</v>
       </c>
       <c r="C33">
-        <v>9.386506999482401e-05</v>
+        <v>8.39048680248166e-05</v>
       </c>
       <c r="D33">
-        <v>-0.1406250051574145</v>
+        <v>-0.140625005180008</v>
       </c>
       <c r="E33">
-        <v>5.8665668746765e-06</v>
+        <v>5.24405425155104e-06</v>
       </c>
       <c r="F33">
         <v>0.0625</v>
@@ -1295,13 +1507,13 @@
         <v>37</v>
       </c>
       <c r="C34">
-        <v>8.390457256522847e-05</v>
+        <v>7.5394947938766e-05</v>
       </c>
       <c r="D34">
-        <v>-0.1406250051800086</v>
+        <v>-0.140625005197306</v>
       </c>
       <c r="E34">
-        <v>5.244035785326779e-06</v>
+        <v>4.71218424617287e-06</v>
       </c>
       <c r="F34">
         <v>0.0625</v>
@@ -1315,13 +1527,13 @@
         <v>38</v>
       </c>
       <c r="C35">
-        <v>7.539457738011352e-05</v>
+        <v>6.81653591912005e-05</v>
       </c>
       <c r="D35">
-        <v>-0.1406250051973067</v>
+        <v>-0.140625005210549</v>
       </c>
       <c r="E35">
-        <v>4.712161086255491e-06</v>
+        <v>4.26033494945003e-06</v>
       </c>
       <c r="F35">
         <v>0.0625</v>
@@ -1335,13 +1547,13 @@
         <v>39</v>
       </c>
       <c r="C36">
-        <v>6.816497805405357e-05</v>
+        <v>6.20638057978422e-05</v>
       </c>
       <c r="D36">
-        <v>-0.1406250052105501</v>
+        <v>-0.140625005220688</v>
       </c>
       <c r="E36">
-        <v>4.260311128378348e-06</v>
+        <v>3.87898786236514e-06</v>
       </c>
       <c r="F36">
         <v>0.0625</v>
@@ -1355,13 +1567,13 @@
         <v>40</v>
       </c>
       <c r="C37">
-        <v>6.206338043275361e-05</v>
+        <v>5.69524352616124e-05</v>
       </c>
       <c r="D37">
-        <v>-0.1406250052206893</v>
+        <v>-0.140625005228451</v>
       </c>
       <c r="E37">
-        <v>3.878961277045145e-06</v>
+        <v>3.55952720385078e-06</v>
       </c>
       <c r="F37">
         <v>0.0625</v>
@@ -1375,13 +1587,13 @@
         <v>41</v>
       </c>
       <c r="C38">
-        <v>5.695188152164678e-05</v>
+        <v>5.27053096150452e-05</v>
       </c>
       <c r="D38">
-        <v>-0.1406250052284518</v>
+        <v>-0.140625005234393</v>
       </c>
       <c r="E38">
-        <v>3.559492595102924e-06</v>
+        <v>3.29408185094032e-06</v>
       </c>
       <c r="F38">
         <v>0.0625</v>
@@ -1395,13 +1607,13 @@
         <v>42</v>
       </c>
       <c r="C39">
-        <v>5.270453824488615e-05</v>
+        <v>4.9206485621055e-05</v>
       </c>
       <c r="D39">
-        <v>-0.1406250052343948</v>
+        <v>-0.140625005238944</v>
       </c>
       <c r="E39">
-        <v>3.294033640303074e-06</v>
+        <v>3.07540535131594e-06</v>
       </c>
       <c r="F39">
         <v>0.0625</v>
@@ -1415,13 +1627,13 @@
         <v>43</v>
       </c>
       <c r="C40">
-        <v>4.920562878463986e-05</v>
+        <v>4.63496055970187e-05</v>
       </c>
       <c r="D40">
-        <v>-0.1406250052389447</v>
+        <v>-0.140625005242427</v>
       </c>
       <c r="E40">
-        <v>3.075351799039991e-06</v>
+        <v>2.89685034981367e-06</v>
       </c>
       <c r="F40">
         <v>0.0625</v>
@@ -1435,13 +1647,13 @@
         <v>44</v>
       </c>
       <c r="C41">
-        <v>4.634872030251271e-05</v>
+        <v>4.40374788161343e-05</v>
       </c>
       <c r="D41">
-        <v>-0.140625005242428</v>
+        <v>-0.140625005245093</v>
       </c>
       <c r="E41">
-        <v>2.896795018904411e-06</v>
+        <v>2.75234242600839e-06</v>
       </c>
       <c r="F41">
         <v>0.0625</v>
@@ -1455,13 +1667,13 @@
         <v>45</v>
       </c>
       <c r="C42">
-        <v>4.403642449043716e-05</v>
+        <v>4.21818680385961e-05</v>
       </c>
       <c r="D42">
-        <v>-0.1406250052450948</v>
+        <v>-0.140625005247135</v>
       </c>
       <c r="E42">
-        <v>2.752276530652323e-06</v>
+        <v>2.63636675241226e-06</v>
       </c>
       <c r="F42">
         <v>0.0625</v>
@@ -1475,13 +1687,13 @@
         <v>46</v>
       </c>
       <c r="C43">
-        <v>4.218059830682092e-05</v>
+        <v>4.07040053995772e-05</v>
       </c>
       <c r="D43">
-        <v>-0.1406250052471364</v>
+        <v>-0.140625005248698</v>
       </c>
       <c r="E43">
-        <v>2.636287394176307e-06</v>
+        <v>2.54400033747358e-06</v>
       </c>
       <c r="F43">
         <v>0.0625</v>
@@ -1495,13 +1707,13 @@
         <v>47</v>
       </c>
       <c r="C44">
-        <v>4.070268733551901e-05</v>
+        <v>3.95352937893122e-05</v>
       </c>
       <c r="D44">
-        <v>-0.1406250052486994</v>
+        <v>-0.140625005249894</v>
       </c>
       <c r="E44">
-        <v>2.543917958469938e-06</v>
+        <v>2.47095586183201e-06</v>
       </c>
       <c r="F44">
         <v>0.0625</v>
@@ -1515,13 +1727,13 @@
         <v>48</v>
       </c>
       <c r="C45">
-        <v>3.953393899013167e-05</v>
+        <v>3.86169458764444e-05</v>
       </c>
       <c r="D45">
-        <v>-0.1406250052498959</v>
+        <v>-0.14062500525081</v>
       </c>
       <c r="E45">
-        <v>2.470871186880132e-06</v>
+        <v>2.41355911727778e-06</v>
       </c>
       <c r="F45">
         <v>0.0625</v>
@@ -1535,13 +1747,13 @@
         <v>49</v>
       </c>
       <c r="C46">
-        <v>3.861531280165623e-05</v>
+        <v>3.78989055682365e-05</v>
       </c>
       <c r="D46">
-        <v>-0.1406250052508119</v>
+        <v>-0.140625005251511</v>
       </c>
       <c r="E46">
-        <v>2.413457050103514e-06</v>
+        <v>2.36868159801478e-06</v>
       </c>
       <c r="F46">
         <v>0.0625</v>
@@ -1555,13 +1767,13 @@
         <v>50</v>
       </c>
       <c r="C47">
-        <v>3.789703733710461e-05</v>
+        <v>3.73398654639271e-05</v>
       </c>
       <c r="D47">
-        <v>-0.1406250052515131</v>
+        <v>-0.140625005252047</v>
       </c>
       <c r="E47">
-        <v>2.368564833569038e-06</v>
+        <v>2.33374159149545e-06</v>
       </c>
       <c r="F47">
         <v>0.0625</v>
@@ -1575,13 +1787,13 @@
         <v>51</v>
       </c>
       <c r="C48">
-        <v>3.733786237613751e-05</v>
+        <v>3.69061456470003e-05</v>
       </c>
       <c r="D48">
-        <v>-0.1406250052520498</v>
+        <v>-0.140625005252458</v>
       </c>
       <c r="E48">
-        <v>2.333616398508594e-06</v>
+        <v>2.30663410293752e-06</v>
       </c>
       <c r="F48">
         <v>0.0625</v>
@@ -1595,13 +1807,13 @@
         <v>52</v>
       </c>
       <c r="C49">
-        <v>3.690410867391916e-05</v>
+        <v>3.65706738486494e-05</v>
       </c>
       <c r="D49">
-        <v>-0.1406250052524607</v>
+        <v>-0.140625005252773</v>
       </c>
       <c r="E49">
-        <v>2.306506792116623e-06</v>
+        <v>2.28566711554059e-06</v>
       </c>
       <c r="F49">
         <v>0.0625</v>
@@ -1615,13 +1827,13 @@
         <v>53</v>
       </c>
       <c r="C50">
-        <v>3.656862804499381e-05</v>
+        <v>3.63119047871202e-05</v>
       </c>
       <c r="D50">
-        <v>-0.1406250052527751</v>
+        <v>-0.140625005253013</v>
       </c>
       <c r="E50">
-        <v>2.285539252812113e-06</v>
+        <v>2.26949404919501e-06</v>
       </c>
       <c r="F50">
         <v>0.0625</v>
@@ -1635,13 +1847,13 @@
         <v>54</v>
       </c>
       <c r="C51">
-        <v>3.63097688355954e-05</v>
+        <v>3.61126561563225e-05</v>
       </c>
       <c r="D51">
-        <v>-0.1406250052530158</v>
+        <v>-0.140625005253197</v>
       </c>
       <c r="E51">
-        <v>2.269360552224712e-06</v>
+        <v>2.25704100977016e-06</v>
       </c>
       <c r="F51">
         <v>0.0625</v>
@@ -1655,13 +1867,13 @@
         <v>55</v>
       </c>
       <c r="C52">
-        <v>3.611041275460737e-05</v>
+        <v>3.59593409443661e-05</v>
       </c>
       <c r="D52">
-        <v>-0.1406250052531999</v>
+        <v>-0.140625005253338</v>
       </c>
       <c r="E52">
-        <v>2.256900797162961e-06</v>
+        <v>2.24745880902288e-06</v>
       </c>
       <c r="F52">
         <v>0.0625</v>
@@ -1675,13 +1887,13 @@
         <v>56</v>
       </c>
       <c r="C53">
-        <v>3.595712019769896e-05</v>
+        <v>3.58415892088112e-05</v>
       </c>
       <c r="D53">
-        <v>-0.1406250052533408</v>
+        <v>-0.140625005253446</v>
       </c>
       <c r="E53">
-        <v>2.24732001235277e-06</v>
+        <v>2.2400993255507e-06</v>
       </c>
       <c r="F53">
         <v>0.0625</v>
@@ -1695,13 +1907,13 @@
         <v>57</v>
       </c>
       <c r="C54">
-        <v>3.583939836993704e-05</v>
+        <v>3.57513955140957e-05</v>
       </c>
       <c r="D54">
-        <v>-0.1406250052534486</v>
+        <v>-0.140625005253528</v>
       </c>
       <c r="E54">
-        <v>2.239962398121065e-06</v>
+        <v>2.23446221963098e-06</v>
       </c>
       <c r="F54">
         <v>0.0625</v>
@@ -1715,13 +1927,13 @@
         <v>58</v>
       </c>
       <c r="C55">
-        <v>3.574909110173323e-05</v>
+        <v>3.56822130447293e-05</v>
       </c>
       <c r="D55">
-        <v>-0.140625005253531</v>
+        <v>-0.140625005253591</v>
       </c>
       <c r="E55">
-        <v>2.234318193858327e-06</v>
+        <v>2.23013831529558e-06</v>
       </c>
       <c r="F55">
         <v>0.0625</v>
@@ -1735,13 +1947,13 @@
         <v>59</v>
       </c>
       <c r="C56">
-        <v>3.567988030685947e-05</v>
+        <v>3.56292047858688e-05</v>
       </c>
       <c r="D56">
-        <v>-0.140625005253594</v>
+        <v>-0.14062500525364</v>
       </c>
       <c r="E56">
-        <v>2.229992519178717e-06</v>
+        <v>2.2268252991168e-06</v>
       </c>
       <c r="F56">
         <v>0.0625</v>
@@ -1755,13 +1967,13 @@
         <v>60</v>
       </c>
       <c r="C57">
-        <v>3.562688486438607e-05</v>
+        <v>3.55887852164099e-05</v>
       </c>
       <c r="D57">
-        <v>-0.1406250052536422</v>
+        <v>-0.140625005253676</v>
       </c>
       <c r="E57">
-        <v>2.226680304024129e-06</v>
+        <v>2.22429907602562e-06</v>
       </c>
       <c r="F57">
         <v>0.0625</v>
@@ -1775,13 +1987,13 @@
         <v>61</v>
       </c>
       <c r="C58">
-        <v>3.558634164333562e-05</v>
+        <v>3.55578615104329e-05</v>
       </c>
       <c r="D58">
-        <v>-0.1406250052536789</v>
+        <v>-0.140625005253704</v>
       </c>
       <c r="E58">
-        <v>2.224146352708476e-06</v>
+        <v>2.22236634440206e-06</v>
       </c>
       <c r="F58">
         <v>0.0625</v>
@@ -1795,13 +2007,13 @@
         <v>62</v>
       </c>
       <c r="C59">
-        <v>3.555535410342774e-05</v>
+        <v>3.55342898802163e-05</v>
       </c>
       <c r="D59">
-        <v>-0.140625005253707</v>
+        <v>-0.140625005253725</v>
       </c>
       <c r="E59">
-        <v>2.222209631464234e-06</v>
+        <v>2.22089311751352e-06</v>
       </c>
       <c r="F59">
         <v>0.0625</v>
@@ -1815,13 +2027,13 @@
         <v>63</v>
       </c>
       <c r="C60">
-        <v>3.553169550151969e-05</v>
+        <v>3.5516298549534e-05</v>
       </c>
       <c r="D60">
-        <v>-0.1406250052537284</v>
+        <v>-0.140625005253742</v>
       </c>
       <c r="E60">
-        <v>2.220730968844981e-06</v>
+        <v>2.21976865934588e-06</v>
       </c>
       <c r="F60">
         <v>0.0625</v>
@@ -1835,13 +2047,13 @@
         <v>64</v>
       </c>
       <c r="C61">
-        <v>3.551365564599032e-05</v>
+        <v>3.55025277202721e-05</v>
       </c>
       <c r="D61">
-        <v>-0.1406250052537447</v>
+        <v>-0.140625005253754</v>
       </c>
       <c r="E61">
-        <v>2.219603477874395e-06</v>
+        <v>2.218907982517e-06</v>
       </c>
       <c r="F61">
         <v>0.0625</v>
@@ -1855,13 +2067,13 @@
         <v>65</v>
       </c>
       <c r="C62">
-        <v>3.549992203371994e-05</v>
+        <v>3.5492200863691e-05</v>
       </c>
       <c r="D62">
-        <v>-0.140625005253757</v>
+        <v>-0.140625005253763</v>
       </c>
       <c r="E62">
-        <v>2.218745127107496e-06</v>
+        <v>2.21826255398069e-06</v>
       </c>
       <c r="F62">
         <v>0.0625</v>
@@ -1875,13 +2087,13 @@
         <v>66</v>
       </c>
       <c r="C63">
-        <v>3.54894879428817e-05</v>
+        <v>3.54843739126142e-05</v>
       </c>
       <c r="D63">
-        <v>-0.1406250052537664</v>
+        <v>-0.14062500525377</v>
       </c>
       <c r="E63">
-        <v>2.218092996430106e-06</v>
+        <v>2.21777336953839e-06</v>
       </c>
       <c r="F63">
         <v>0.0625</v>
@@ -1895,13 +2107,13 @@
         <v>67</v>
       </c>
       <c r="C64">
-        <v>3.548158152827225e-05</v>
+        <v>3.54784275338752e-05</v>
       </c>
       <c r="D64">
-        <v>-0.1406250052537735</v>
+        <v>-0.140625005253776</v>
       </c>
       <c r="E64">
-        <v>2.217598845517015e-06</v>
+        <v>2.2174017208672e-06</v>
       </c>
       <c r="F64">
         <v>0.0625</v>
@@ -1915,13 +2127,13 @@
         <v>68</v>
       </c>
       <c r="C65">
-        <v>3.547561121961182e-05</v>
+        <v>3.54740155504928e-05</v>
       </c>
       <c r="D65">
-        <v>-0.1406250052537788</v>
+        <v>-0.14062500525378</v>
       </c>
       <c r="E65">
-        <v>2.217225701222273e-06</v>
+        <v>2.2171259719058e-06</v>
       </c>
       <c r="F65">
         <v>0.0625</v>
@@ -1935,13 +2147,13 @@
         <v>69</v>
       </c>
       <c r="C66">
-        <v>3.54711237322188e-05</v>
+        <v>3.54707700621946e-05</v>
       </c>
       <c r="D66">
-        <v>-0.1406250052537828</v>
+        <v>-0.140625005253782</v>
       </c>
       <c r="E66">
-        <v>2.216945233263675e-06</v>
+        <v>2.21692312888716e-06</v>
       </c>
       <c r="F66">
         <v>0.0625</v>
@@ -1955,13 +2167,13 @@
         <v>70</v>
       </c>
       <c r="C67">
-        <v>3.546777180825175e-05</v>
+        <v>3.54682700344688e-05</v>
       </c>
       <c r="D67">
-        <v>-0.1406250052537858</v>
+        <v>-0.140625005253785</v>
       </c>
       <c r="E67">
-        <v>2.216735738012267e-06</v>
+        <v>2.2167668771543e-06</v>
       </c>
       <c r="F67">
         <v>0.0625</v>
@@ -1975,13 +2187,13 @@
         <v>71</v>
       </c>
       <c r="C68">
-        <v>3.54652894569018e-05</v>
+        <v>3.54664304306014e-05</v>
       </c>
       <c r="D68">
-        <v>-0.1406250052537879</v>
+        <v>-0.140625005253786</v>
       </c>
       <c r="E68">
-        <v>2.216580591056363e-06</v>
+        <v>2.21665190191259e-06</v>
       </c>
       <c r="F68">
         <v>0.0625</v>
@@ -1995,13 +2207,13 @@
         <v>72</v>
       </c>
       <c r="C69">
-        <v>3.546347296021305e-05</v>
+        <v>3.54652134682088e-05</v>
       </c>
       <c r="D69">
-        <v>-0.1406250052537895</v>
+        <v>-0.140625005253787</v>
       </c>
       <c r="E69">
-        <v>2.216467060013316e-06</v>
+        <v>2.21657584176305e-06</v>
       </c>
       <c r="F69">
         <v>0.0625</v>
@@ -2015,13 +2227,13 @@
         <v>73</v>
       </c>
       <c r="C70">
-        <v>3.546216630602487e-05</v>
+        <v>3.54643484395637e-05</v>
       </c>
       <c r="D70">
-        <v>-0.1406250052537906</v>
+        <v>-0.140625005253788</v>
       </c>
       <c r="E70">
-        <v>2.216385394126555e-06</v>
+        <v>2.21652177747273e-06</v>
       </c>
       <c r="F70">
         <v>0.0625</v>
@@ -2035,13 +2247,13 @@
         <v>74</v>
       </c>
       <c r="C71">
-        <v>3.546125002436757e-05</v>
+        <v>3.54638699983641e-05</v>
       </c>
       <c r="D71">
-        <v>-0.1406250052537914</v>
+        <v>-0.140625005253788</v>
       </c>
       <c r="E71">
-        <v>2.216328126519504e-06</v>
+        <v>2.21649187489775e-06</v>
       </c>
       <c r="F71">
         <v>0.0625</v>
@@ -2055,13 +2267,13 @@
         <v>75</v>
       </c>
       <c r="C72">
-        <v>3.546063263488686e-05</v>
+        <v>3.54635576293286e-05</v>
       </c>
       <c r="D72">
-        <v>-0.1406250052537919</v>
+        <v>-0.140625005253789</v>
       </c>
       <c r="E72">
-        <v>2.216289539680429e-06</v>
+        <v>2.21647235183304e-06</v>
       </c>
       <c r="F72">
         <v>0.0625</v>
@@ -2075,13 +2287,13 @@
         <v>76</v>
       </c>
       <c r="C73">
-        <v>3.546024409137433e-05</v>
+        <v>3.54633499722813e-05</v>
       </c>
       <c r="D73">
-        <v>-0.1406250052537922</v>
+        <v>-0.140625005253789</v>
       </c>
       <c r="E73">
-        <v>2.216265255710895e-06</v>
+        <v>2.21645937326758e-06</v>
       </c>
       <c r="F73">
         <v>0.0625</v>
@@ -2095,16 +2307,16 @@
         <v>77</v>
       </c>
       <c r="C74">
-        <v>3.546003075982554e-05</v>
+        <v>3.54633353135669e-05</v>
       </c>
       <c r="D74">
-        <v>-0.1406250052537923</v>
+        <v>-0.140625005273439</v>
       </c>
       <c r="E74">
-        <v>2.216251922489096e-06</v>
+        <v>1.10822922854897e-06</v>
       </c>
       <c r="F74">
-        <v>0.0625</v>
+        <v>0.03125</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -2115,56 +2327,16 @@
         <v>78</v>
       </c>
       <c r="C75">
-        <v>3.545995157575033e-05</v>
+        <v>1.98496032207886e-08</v>
       </c>
       <c r="D75">
-        <v>-0.1406250052537923</v>
+        <v>-0.140625005273439</v>
       </c>
       <c r="E75">
-        <v>2.216246973487864e-06</v>
+        <v>1.24060020129929e-09</v>
       </c>
       <c r="F75">
         <v>0.0625</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6">
-      <c r="A76" s="1">
-        <v>74</v>
-      </c>
-      <c r="B76" t="s">
-        <v>79</v>
-      </c>
-      <c r="C76">
-        <v>3.545997509911307e-05</v>
-      </c>
-      <c r="D76">
-        <v>-0.1406250052734393</v>
-      </c>
-      <c r="E76">
-        <v>1.108124221849018e-06</v>
-      </c>
-      <c r="F76">
-        <v>0.03125</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
-      <c r="A77" s="1">
-        <v>75</v>
-      </c>
-      <c r="B77" t="s">
-        <v>80</v>
-      </c>
-      <c r="C77">
-        <v>1.74248403165024e-08</v>
-      </c>
-      <c r="D77">
-        <v>-0.1406250052734392</v>
-      </c>
-      <c r="E77">
-        <v>2.1781050395628e-09</v>
-      </c>
-      <c r="F77">
-        <v>0.125</v>
       </c>
     </row>
   </sheetData>
@@ -2173,6 +2345,1376 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F68"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2">
+        <v>1.4142135623731</v>
+      </c>
+      <c r="D2">
+        <v>-0.0555555555554748</v>
+      </c>
+      <c r="E2">
+        <v>0.0785673254111343</v>
+      </c>
+      <c r="F2">
+        <v>0.0555554885779032</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3">
+        <v>1.09994301036729</v>
+      </c>
+      <c r="D3">
+        <v>-0.0891632033608961</v>
+      </c>
+      <c r="E3">
+        <v>0.0611079450204107</v>
+      </c>
+      <c r="F3">
+        <v>0.0555555555555606</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4">
+        <v>0.855512803206276</v>
+      </c>
+      <c r="D4">
+        <v>-0.109493754520291</v>
+      </c>
+      <c r="E4">
+        <v>0.0475283171662895</v>
+      </c>
+      <c r="F4">
+        <v>0.0555553546225886</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5">
+        <v>0.665398360380009</v>
+      </c>
+      <c r="D5">
+        <v>-0.121792490846486</v>
+      </c>
+      <c r="E5">
+        <v>0.0369665087264321</v>
+      </c>
+      <c r="F5">
+        <v>0.0555554550890696</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6">
+        <v>0.517533013784635</v>
+      </c>
+      <c r="D6">
+        <v>-0.129232475705279</v>
+      </c>
+      <c r="E6">
+        <v>0.0287516954465536</v>
+      </c>
+      <c r="F6">
+        <v>0.0555552876449313</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7">
+        <v>0.402525435211076</v>
+      </c>
+      <c r="D7">
+        <v>-0.133733214164321</v>
+      </c>
+      <c r="E7">
+        <v>0.0223624702579738</v>
+      </c>
+      <c r="F7">
+        <v>0.0555554216002459</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8">
+        <v>0.313076034670962</v>
+      </c>
+      <c r="D8">
+        <v>-0.136455888021673</v>
+      </c>
+      <c r="E8">
+        <v>0.0173930291608798</v>
+      </c>
+      <c r="F8">
+        <v>0.0555552876449313</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9">
+        <v>0.243503611207976</v>
+      </c>
+      <c r="D9">
+        <v>-0.138102940946394</v>
+      </c>
+      <c r="E9">
+        <v>0.0135279457818415</v>
+      </c>
+      <c r="F9">
+        <v>0.0555554216002459</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10">
+        <v>0.189392219112291</v>
+      </c>
+      <c r="D10">
+        <v>-0.139099308445566</v>
+      </c>
+      <c r="E10">
+        <v>0.010521726525448</v>
+      </c>
+      <c r="F10">
+        <v>0.0555552206672739</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11">
+        <v>0.147304956295077</v>
+      </c>
+      <c r="D11">
+        <v>-0.139702050644825</v>
+      </c>
+      <c r="E11">
+        <v>0.00818358895077881</v>
+      </c>
+      <c r="F11">
+        <v>0.0555554216002459</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12">
+        <v>0.114570869785469</v>
+      </c>
+      <c r="D12">
+        <v>-0.140066673324687</v>
+      </c>
+      <c r="E12">
+        <v>0.00636500995297327</v>
+      </c>
+      <c r="F12">
+        <v>0.0555552206672739</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13">
+        <v>0.089110633165834</v>
+      </c>
+      <c r="D13">
+        <v>-0.140287248069973</v>
+      </c>
+      <c r="E13">
+        <v>0.00495058177880305</v>
+      </c>
+      <c r="F13">
+        <v>0.0555554550890696</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14">
+        <v>0.0693085332443209</v>
+      </c>
+      <c r="D14">
+        <v>-0.140420682502517</v>
+      </c>
+      <c r="E14">
+        <v>0.00385044157426697</v>
+      </c>
+      <c r="F14">
+        <v>0.0555550867119593</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15">
+        <v>0.0539064865217174</v>
+      </c>
+      <c r="D15">
+        <v>-0.140501402297272</v>
+      </c>
+      <c r="E15">
+        <v>0.00299480480676235</v>
+      </c>
+      <c r="F15">
+        <v>0.0555555555555606</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16">
+        <v>0.0419275057791861</v>
+      </c>
+      <c r="D16">
+        <v>-0.140550232912845</v>
+      </c>
+      <c r="E16">
+        <v>0.00232928762328171</v>
+      </c>
+      <c r="F16">
+        <v>0.055555120200783</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17">
+        <v>0.0326102129046779</v>
+      </c>
+      <c r="D17">
+        <v>-0.140579772495511</v>
+      </c>
+      <c r="E17">
+        <v>0.00181167412639316</v>
+      </c>
+      <c r="F17">
+        <v>0.0555554216002459</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18">
+        <v>0.025363583418921</v>
+      </c>
+      <c r="D18">
+        <v>-0.140597642165131</v>
+      </c>
+      <c r="E18">
+        <v>0.00140908117254436</v>
+      </c>
+      <c r="F18">
+        <v>0.0555552876449313</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19">
+        <v>0.019727249715961</v>
+      </c>
+      <c r="D19">
+        <v>-0.140608452239605</v>
+      </c>
+      <c r="E19">
+        <v>0.00109595038984367</v>
+      </c>
+      <c r="F19">
+        <v>0.0555551536896166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20">
+        <v>0.0153433939401628</v>
+      </c>
+      <c r="D20">
+        <v>-0.140614991684054</v>
+      </c>
+      <c r="E20">
+        <v>0.000852411802118156</v>
+      </c>
+      <c r="F20">
+        <v>0.0555556225332179</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21">
+        <v>0.0119338341347936</v>
+      </c>
+      <c r="D21">
+        <v>-0.140618947654448</v>
+      </c>
+      <c r="E21">
+        <v>0.000662982792263845</v>
+      </c>
+      <c r="F21">
+        <v>0.0555548857789873</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22">
+        <v>0.00928181250571941</v>
+      </c>
+      <c r="D22">
+        <v>-0.140621340778469</v>
+      </c>
+      <c r="E22">
+        <v>0.000515658426176957</v>
+      </c>
+      <c r="F22">
+        <v>0.0555557899773562</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>100</v>
+      </c>
+      <c r="C23">
+        <v>0.00721925968753133</v>
+      </c>
+      <c r="D23">
+        <v>-0.140622788474478</v>
+      </c>
+      <c r="E23">
+        <v>0.000401063454997764</v>
+      </c>
+      <c r="F23">
+        <v>0.0555546513571817</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24">
+        <v>0.00561492086165434</v>
+      </c>
+      <c r="D24">
+        <v>-0.140623664243459</v>
+      </c>
+      <c r="E24">
+        <v>0.000311943056463687</v>
+      </c>
+      <c r="F24">
+        <v>0.0555560913768192</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25">
+        <v>0.00436722814824531</v>
+      </c>
+      <c r="D25">
+        <v>-0.140624194031011</v>
+      </c>
+      <c r="E25">
+        <v>0.000242617350866025</v>
+      </c>
+      <c r="F25">
+        <v>0.0555540820470994</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26">
+        <v>0.00339666241855157</v>
+      </c>
+      <c r="D26">
+        <v>-0.140624514520571</v>
+      </c>
+      <c r="E26">
+        <v>0.000188705970202742</v>
+      </c>
+      <c r="F26">
+        <v>0.0555562923097911</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27">
+        <v>0.00264189901982175</v>
+      </c>
+      <c r="D27">
+        <v>-0.140624708397482</v>
+      </c>
+      <c r="E27">
+        <v>0.000146769425070656</v>
+      </c>
+      <c r="F27">
+        <v>0.055554517401867</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28">
+        <v>0.00205478389226967</v>
+      </c>
+      <c r="D28">
+        <v>-0.140624825681338</v>
+      </c>
+      <c r="E28">
+        <v>0.000114155968115463</v>
+      </c>
+      <c r="F28">
+        <v>0.0555561918433001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29">
+        <v>0.00159819274976281</v>
+      </c>
+      <c r="D29">
+        <v>-0.140624896631025</v>
+      </c>
+      <c r="E29">
+        <v>8.87849536721336e-05</v>
+      </c>
+      <c r="F29">
+        <v>0.0555533452928688</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30">
+        <v>0.00124299653260691</v>
+      </c>
+      <c r="D30">
+        <v>-0.140624939551316</v>
+      </c>
+      <c r="E30">
+        <v>6.90589011749316e-05</v>
+      </c>
+      <c r="F30">
+        <v>0.0555584021059919</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31">
+        <v>0.000966830153778909</v>
+      </c>
+      <c r="D31">
+        <v>-0.140624965515511</v>
+      </c>
+      <c r="E31">
+        <v>5.37083181557599e-05</v>
+      </c>
+      <c r="F31">
+        <v>0.0555509340972051</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>109</v>
+      </c>
+      <c r="C32">
+        <v>0.000751920821730178</v>
+      </c>
+      <c r="D32">
+        <v>-0.140624981222283</v>
+      </c>
+      <c r="E32">
+        <v>4.17773827556661e-05</v>
+      </c>
+      <c r="F32">
+        <v>0.0555608802793129</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>110</v>
+      </c>
+      <c r="C33">
+        <v>0.000584886786453171</v>
+      </c>
+      <c r="D33">
+        <v>-0.140624990723937</v>
+      </c>
+      <c r="E33">
+        <v>3.24905568235886e-05</v>
+      </c>
+      <c r="F33">
+        <v>0.0555501638541409</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34">
+        <v>0.000454870357701679</v>
+      </c>
+      <c r="D34">
+        <v>-0.140624996471866</v>
+      </c>
+      <c r="E34">
+        <v>2.52723729307878e-05</v>
+      </c>
+      <c r="F34">
+        <v>0.0555595072373427</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>112</v>
+      </c>
+      <c r="C35">
+        <v>0.000353815340588616</v>
+      </c>
+      <c r="D35">
+        <v>-0.140624999949015</v>
+      </c>
+      <c r="E35">
+        <v>1.96532323156451e-05</v>
+      </c>
+      <c r="F35">
+        <v>0.055546580549479</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>113</v>
+      </c>
+      <c r="C36">
+        <v>0.00027514694587358</v>
+      </c>
+      <c r="D36">
+        <v>-0.140625002052483</v>
+      </c>
+      <c r="E36">
+        <v>1.52888716003846e-05</v>
+      </c>
+      <c r="F36">
+        <v>0.0555662050030753</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>114</v>
+      </c>
+      <c r="C37">
+        <v>0.000214045481047597</v>
+      </c>
+      <c r="D37">
+        <v>-0.140625003324956</v>
+      </c>
+      <c r="E37">
+        <v>1.18899676510119e-05</v>
+      </c>
+      <c r="F37">
+        <v>0.0555487908121707</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>115</v>
+      </c>
+      <c r="C38">
+        <v>0.000166460424722525</v>
+      </c>
+      <c r="D38">
+        <v>-0.140625004094723</v>
+      </c>
+      <c r="E38">
+        <v>9.24698748703346e-06</v>
+      </c>
+      <c r="F38">
+        <v>0.0555506661865758</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>116</v>
+      </c>
+      <c r="C39">
+        <v>0.000129458689793119</v>
+      </c>
+      <c r="D39">
+        <v>-0.140625004560387</v>
+      </c>
+      <c r="E39">
+        <v>7.19279107509425e-06</v>
+      </c>
+      <c r="F39">
+        <v>0.0555605119022026</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>117</v>
+      </c>
+      <c r="C40">
+        <v>0.00010069970907973</v>
+      </c>
+      <c r="D40">
+        <v>-0.140625004842086</v>
+      </c>
+      <c r="E40">
+        <v>5.59339972603243e-06</v>
+      </c>
+      <c r="F40">
+        <v>0.0555453414628135</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41">
+        <v>7.83079774316163e-05</v>
+      </c>
+      <c r="D41">
+        <v>-0.140625005012496</v>
+      </c>
+      <c r="E41">
+        <v>4.35032255829959e-06</v>
+      </c>
+      <c r="F41">
+        <v>0.0555540150694421</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42">
+        <v>6.09050179430415e-05</v>
+      </c>
+      <c r="D42">
+        <v>-0.140625005115584</v>
+      </c>
+      <c r="E42">
+        <v>3.38438309100003e-06</v>
+      </c>
+      <c r="F42">
+        <v>0.055568214332795</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43">
+        <v>4.73816354095425e-05</v>
+      </c>
+      <c r="D43">
+        <v>-0.140625005177946</v>
+      </c>
+      <c r="E43">
+        <v>2.63340476606664e-06</v>
+      </c>
+      <c r="F43">
+        <v>0.0555785958696804</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>121</v>
+      </c>
+      <c r="C44">
+        <v>3.68679918912728e-05</v>
+      </c>
+      <c r="D44">
+        <v>-0.140625005215672</v>
+      </c>
+      <c r="E44">
+        <v>2.04592035456751e-06</v>
+      </c>
+      <c r="F44">
+        <v>0.0554931323789335</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>122</v>
+      </c>
+      <c r="C45">
+        <v>2.86430008831276e-05</v>
+      </c>
+      <c r="D45">
+        <v>-0.140625005238493</v>
+      </c>
+      <c r="E45">
+        <v>1.59167302570549e-06</v>
+      </c>
+      <c r="F45">
+        <v>0.0555693529529696</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>123</v>
+      </c>
+      <c r="C46">
+        <v>2.22834021578362e-05</v>
+      </c>
+      <c r="D46">
+        <v>-0.140625005252299</v>
+      </c>
+      <c r="E46">
+        <v>1.23785261105057e-06</v>
+      </c>
+      <c r="F46">
+        <v>0.0555504317647702</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>124</v>
+      </c>
+      <c r="C47">
+        <v>1.73298580018302e-05</v>
+      </c>
+      <c r="D47">
+        <v>-0.140625005260651</v>
+      </c>
+      <c r="E47">
+        <v>9.62392657164434e-07</v>
+      </c>
+      <c r="F47">
+        <v>0.0555337878169299</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>125</v>
+      </c>
+      <c r="C48">
+        <v>1.34735409538681e-05</v>
+      </c>
+      <c r="D48">
+        <v>-0.140625005265703</v>
+      </c>
+      <c r="E48">
+        <v>7.48361299286933e-07</v>
+      </c>
+      <c r="F48">
+        <v>0.0555430307336408</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>126</v>
+      </c>
+      <c r="C49">
+        <v>1.04771571449638e-05</v>
+      </c>
+      <c r="D49">
+        <v>-0.140625005268759</v>
+      </c>
+      <c r="E49">
+        <v>5.81784293380563e-07</v>
+      </c>
+      <c r="F49">
+        <v>0.0555288314702878</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>127</v>
+      </c>
+      <c r="C50">
+        <v>8.14503831398092e-06</v>
+      </c>
+      <c r="D50">
+        <v>-0.140625005270608</v>
+      </c>
+      <c r="E50">
+        <v>4.53245148017842e-07</v>
+      </c>
+      <c r="F50">
+        <v>0.0556467791248374</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>128</v>
+      </c>
+      <c r="C51">
+        <v>6.34555993471727e-06</v>
+      </c>
+      <c r="D51">
+        <v>-0.140625005271727</v>
+      </c>
+      <c r="E51">
+        <v>3.50873565610949e-07</v>
+      </c>
+      <c r="F51">
+        <v>0.0552943426919924</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>129</v>
+      </c>
+      <c r="C52">
+        <v>4.91232073852142e-06</v>
+      </c>
+      <c r="D52">
+        <v>-0.140625005272403</v>
+      </c>
+      <c r="E52">
+        <v>2.73624620023443e-07</v>
+      </c>
+      <c r="F52">
+        <v>0.0557017008038441</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>130</v>
+      </c>
+      <c r="C53">
+        <v>3.83072277936573e-06</v>
+      </c>
+      <c r="D53">
+        <v>-0.140625005272812</v>
+      </c>
+      <c r="E53">
+        <v>2.12092344199854e-07</v>
+      </c>
+      <c r="F53">
+        <v>0.055366142740645</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>131</v>
+      </c>
+      <c r="C54">
+        <v>2.96937359300943e-06</v>
+      </c>
+      <c r="D54">
+        <v>-0.14062500527306</v>
+      </c>
+      <c r="E54">
+        <v>1.66051292507574e-07</v>
+      </c>
+      <c r="F54">
+        <v>0.0559213205422132</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>132</v>
+      </c>
+      <c r="C55">
+        <v>2.32447229304813e-06</v>
+      </c>
+      <c r="D55">
+        <v>-0.14062500527321</v>
+      </c>
+      <c r="E55">
+        <v>1.27115121970884e-07</v>
+      </c>
+      <c r="F55">
+        <v>0.0546855827645641</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>133</v>
+      </c>
+      <c r="C56">
+        <v>1.7797649579175e-06</v>
+      </c>
+      <c r="D56">
+        <v>-0.140625005273301</v>
+      </c>
+      <c r="E56">
+        <v>1.00787513368992e-07</v>
+      </c>
+      <c r="F56">
+        <v>0.0566296762460841</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>134</v>
+      </c>
+      <c r="C57">
+        <v>1.41018595714114e-06</v>
+      </c>
+      <c r="D57">
+        <v>-0.140625005273355</v>
+      </c>
+      <c r="E57">
+        <v>7.58201237521842e-08</v>
+      </c>
+      <c r="F57">
+        <v>0.053766046507147</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>135</v>
+      </c>
+      <c r="C58">
+        <v>1.0618586869936e-06</v>
+      </c>
+      <c r="D58">
+        <v>-0.140625005273389</v>
+      </c>
+      <c r="E58">
+        <v>6.13160216575064e-08</v>
+      </c>
+      <c r="F58">
+        <v>0.0577440505086601</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>136</v>
+      </c>
+      <c r="C59">
+        <v>8.56258900448143e-07</v>
+      </c>
+      <c r="D59">
+        <v>-0.140625005273409</v>
+      </c>
+      <c r="E59">
+        <v>4.72339239956059e-08</v>
+      </c>
+      <c r="F59">
+        <v>0.0551631334612925</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="1">
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
+        <v>137</v>
+      </c>
+      <c r="C60">
+        <v>6.6121934251002e-07</v>
+      </c>
+      <c r="D60">
+        <v>-0.140625005273421</v>
+      </c>
+      <c r="E60">
+        <v>3.62212996360132e-08</v>
+      </c>
+      <c r="F60">
+        <v>0.0547795524177913</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="1">
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
+        <v>138</v>
+      </c>
+      <c r="C61">
+        <v>5.07313424157616e-07</v>
+      </c>
+      <c r="D61">
+        <v>-0.140625005273428</v>
+      </c>
+      <c r="E61">
+        <v>2.83427934725857e-08</v>
+      </c>
+      <c r="F61">
+        <v>0.0558684081929264</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="1">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
+        <v>139</v>
+      </c>
+      <c r="C62">
+        <v>3.9676546801806e-07</v>
+      </c>
+      <c r="D62">
+        <v>-0.140625005273432</v>
+      </c>
+      <c r="E62">
+        <v>2.12619289311087e-08</v>
+      </c>
+      <c r="F62">
+        <v>0.0535881538492913</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="1">
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>140</v>
+      </c>
+      <c r="C63">
+        <v>2.98200432816358e-07</v>
+      </c>
+      <c r="D63">
+        <v>-0.140625005273435</v>
+      </c>
+      <c r="E63">
+        <v>1.66464619365774e-08</v>
+      </c>
+      <c r="F63">
+        <v>0.0558230643189172</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="1">
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
+        <v>141</v>
+      </c>
+      <c r="C64">
+        <v>2.32861381016962e-07</v>
+      </c>
+      <c r="D64">
+        <v>-0.140625005273437</v>
+      </c>
+      <c r="E64">
+        <v>1.22128625799527e-08</v>
+      </c>
+      <c r="F64">
+        <v>0.052446921546128</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>142</v>
+      </c>
+      <c r="C65">
+        <v>1.72778235270796e-07</v>
+      </c>
+      <c r="D65">
+        <v>-0.140625005273438</v>
+      </c>
+      <c r="E65">
+        <v>9.62834645383473e-09</v>
+      </c>
+      <c r="F65">
+        <v>0.055726616492369</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
+        <v>143</v>
+      </c>
+      <c r="C66">
+        <v>1.34644940673622e-07</v>
+      </c>
+      <c r="D66">
+        <v>-0.140625005273438</v>
+      </c>
+      <c r="E66">
+        <v>8.59656565680248e-09</v>
+      </c>
+      <c r="F66">
+        <v>0.0638461839345834</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>144</v>
+      </c>
+      <c r="C67">
+        <v>1.1709391172723e-07</v>
+      </c>
+      <c r="D67">
+        <v>-0.140625005273439</v>
+      </c>
+      <c r="E67">
+        <v>4.97484460535923e-09</v>
+      </c>
+      <c r="F67">
+        <v>0.042485937371073</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
+        <v>145</v>
+      </c>
+      <c r="C68">
+        <v>7.2387264890264e-08</v>
+      </c>
+      <c r="D68">
+        <v>-0.140625005273439</v>
+      </c>
+      <c r="E68">
+        <v>6.29488667256972e-09</v>
+      </c>
+      <c r="F68">
+        <v>0.0869612451200129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -2202,19 +3744,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>146</v>
       </c>
       <c r="C2">
-        <v>1.414213562373095</v>
+        <v>1.4142135623731</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>-0.140625000000001</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.251945554555299</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2222,16 +3764,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>147</v>
       </c>
       <c r="C3">
-        <v>1.414213562373095</v>
+        <v>0.000562499907763752</v>
       </c>
       <c r="D3">
-        <v>-0.1406250010019531</v>
+        <v>-0.140625005273437</v>
       </c>
       <c r="E3">
-        <v>0.2519455546413066</v>
+        <v>1.87511056627621e-05</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -2242,16 +3784,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>148</v>
       </c>
       <c r="C4">
-        <v>0.0005062500011252634</v>
+        <v>3.39271780300899e-07</v>
       </c>
       <c r="D4">
-        <v>-0.1406250052734379</v>
+        <v>-0.140625005273439</v>
       </c>
       <c r="E4">
-        <v>1.687500009624901e-05</v>
+        <v>1.06085482089284e-08</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -2262,19 +3804,129 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>149</v>
       </c>
       <c r="C5">
-        <v>3.037500017431101e-07</v>
+        <v>1.38777878078145e-10</v>
       </c>
       <c r="D5">
-        <v>-0.1406250052734393</v>
+        <v>-0.140625005273439</v>
       </c>
       <c r="E5">
-        <v>9.492187604328572e-09</v>
+        <v>4.62705904068716e-12</v>
       </c>
       <c r="F5">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2">
+        <v>1.4142135623731</v>
+      </c>
+      <c r="D2">
+        <v>-0.140624999999999</v>
+      </c>
+      <c r="E2">
+        <v>0.251945520805854</v>
+      </c>
+      <c r="F2">
+        <v>0.99999986604469</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3">
+        <v>0.000562499800935951</v>
+      </c>
+      <c r="D3">
+        <v>-0.140625005273437</v>
+      </c>
+      <c r="E3">
+        <v>1.87498878277005e-05</v>
+      </c>
+      <c r="F3">
+        <v>0.999748632852064</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4">
+        <v>3.37674012402159e-07</v>
+      </c>
+      <c r="D4">
+        <v>-0.140625005273439</v>
+      </c>
+      <c r="E4">
+        <v>8.64883544241568e-09</v>
+      </c>
+      <c r="F4">
+        <v>0.819657433394744</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5">
+        <v>6.09293364661224e-08</v>
+      </c>
+      <c r="D5">
+        <v>-0.140625005273439</v>
+      </c>
+      <c r="E5">
+        <v>1.38685942431764e-09</v>
+      </c>
+      <c r="F5">
+        <v>0.728297899473507</v>
       </c>
     </row>
   </sheetData>

</xml_diff>